<commit_message>
new diseases and normalized
</commit_message>
<xml_diff>
--- a/project/excel/dppkb.xlsx
+++ b/project/excel/dppkb.xlsx
@@ -18,15 +18,16 @@
     <sheet name="Genetic" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="Environmental" sheetId="10" state="visible" r:id="rId10"/>
     <sheet name="Disease" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Treatment" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="InfectiousAgent" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="Transmission" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Assay" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Diagnosis" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Inheritance" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="Variant" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="Mechanism" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="DiseaseCollection" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="AnimalModel" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Treatment" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="InfectiousAgent" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Transmission" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Assay" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Diagnosis" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Inheritance" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Variant" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Mechanism" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="DiseaseCollection" sheetId="21" state="visible" r:id="rId21"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -622,12 +623,12 @@
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>treatment</t>
+          <t>inheritance</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>inheritance</t>
+          <t>animal_models</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
@@ -658,6 +659,72 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>species</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>genotype</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>background</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>genes</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>alleles</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>associated_phenotypes</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>name</t>
         </is>
       </c>
@@ -673,36 +740,200 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>context</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>review_notes</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>role</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>mechanism</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>evidence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>evidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>review_notes</t>
+          <t>effect</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>presence</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>evidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>notes</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>results</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>mechanism</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>markers</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -728,201 +959,6 @@
         </is>
       </c>
       <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>evidence</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>effect</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>presence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>evidence</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>notes</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>results</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>markers</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>evidence</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -1029,6 +1065,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1101,7 +1168,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1128,6 +1195,11 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>evidence</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notes</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1290,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1269,55 +1341,60 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>synonyms</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>consequence</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>gene</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>pathways</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>downstream</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>genes</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>subtypes</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>cellular_components</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>chemical_entities</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>triggers</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>assays</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>mechanisms</t>
         </is>
@@ -1334,16 +1411,13 @@
     <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>""</formula1>
     </dataValidation>
-    <dataValidation sqref="J2:J1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>""</formula1>
-    </dataValidation>
     <dataValidation sqref="K2:K1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>""</formula1>
     </dataValidation>
-    <dataValidation sqref="M2:M1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="L2:L1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>""</formula1>
     </dataValidation>
-    <dataValidation sqref="O2:O1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+    <dataValidation sqref="N2:N1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>""</formula1>
     </dataValidation>
     <dataValidation sqref="P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
@@ -1355,6 +1429,9 @@
     <dataValidation sqref="R2:R1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>""</formula1>
     </dataValidation>
+    <dataValidation sqref="S2:S1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>